<commit_message>
updating the data retrieval process in the framework
</commit_message>
<xml_diff>
--- a/Testdata/Naukri_test_data.xlsx
+++ b/Testdata/Naukri_test_data.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\chk017\Eclipse_Projects\ckSampleProject\Testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DB599E-97CE-4C1F-B639-495717F52E7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{51A0544D-118C-468B-9AC1-76FAE9446B2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6225" yWindow="3780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13410" windowHeight="7290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -40,10 +36,10 @@
     <t>naukriupdate</t>
   </si>
   <si>
-    <t>username@gmail.com</t>
+    <t>user@gmail.com</t>
   </si>
   <si>
-    <t>Pass123</t>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -487,7 +483,7 @@
   <dimension ref="A1:IV4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update of dependancies and more ...
</commit_message>
<xml_diff>
--- a/Testdata/Naukri_test_data.xlsx
+++ b/Testdata/Naukri_test_data.xlsx
@@ -1,9 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{51A0544D-118C-468B-9AC1-76FAE9446B2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chk017\eclipse-workspace\CKSelenium\Testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BBD783-D41F-44FE-B832-68F5227B74E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13410" windowHeight="7290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -36,7 +40,7 @@
     <t>naukriupdate</t>
   </si>
   <si>
-    <t>user@gmail.com</t>
+    <t>username@email.com</t>
   </si>
   <si>
     <t>password</t>
@@ -90,12 +94,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -519,7 +524,7 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>